<commit_message>
Frontend: scaffolding the orders page
</commit_message>
<xml_diff>
--- a/WorkBot/main/backend/ordering/Completed Orders/Webstaurant/Webstaurant_Triphammer_20250622.xlsx
+++ b/WorkBot/main/backend/ordering/Completed Orders/Webstaurant/Webstaurant_Triphammer_20250622.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,87 +475,6 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>301SBTG3W</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Tamper Evident - 3 Compartment with Well</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>167.98</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>335.96</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>301SBTGRL</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Lid Tamper Evident - 3 Compartment</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>59.85</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>119.70</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>760RD5</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Container - Alur Deli (5oz)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>97.99</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>97.99</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>